<commit_message>
notas de aula 4 e 5
</commit_message>
<xml_diff>
--- a/DS-PY-Data-Science/DS-PY-004 TÉCNICAS DE PROGRAMAÇÃO I (PY)/Material do Aluno/Aula 4/selic.xlsx
+++ b/DS-PY-Data-Science/DS-PY-004 TÉCNICAS DE PROGRAMAÇÃO I (PY)/Material do Aluno/Aula 4/selic.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="selic" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -6305,7 +6305,7 @@
         </is>
       </c>
       <c r="C452" t="n">
-        <v>0.14</v>
+        <v>0.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>